<commit_message>
added formulas to calculate best-sellers
</commit_message>
<xml_diff>
--- a/Datasets/10567_pev_sales.xlsx
+++ b/Datasets/10567_pev_sales.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Mihok\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Mihok\Desktop\GTBC\GitHub\Team9\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84887036-35B4-4E92-90A5-1332A8CF3317}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD24487-DBC4-43DC-A623-B604A9F32A2A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5685" yWindow="3690" windowWidth="23145" windowHeight="11310" tabRatio="733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PEV Sales Final 2017" sheetId="18" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PEV Sales Final 2017'!$B$3:$K$50</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="69">
   <si>
     <t>Honda Accord</t>
   </si>
@@ -237,6 +237,21 @@
   </si>
   <si>
     <t>Vehicle</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>MAX2011</t>
+  </si>
+  <si>
+    <t>VOLT</t>
+  </si>
+  <si>
+    <t>LEAF</t>
+  </si>
+  <si>
+    <t>TESLA S</t>
   </si>
 </sst>
 </file>
@@ -1155,7 +1170,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1239,6 +1254,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="164">
     <cellStyle name="20% - Accent1 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -5382,7 +5398,7 @@
   <dimension ref="B1:BD62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="S48" sqref="S48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6641,6 +6657,13 @@
         <f t="shared" si="0"/>
         <v>65702</v>
       </c>
+      <c r="L44" t="s">
+        <v>64</v>
+      </c>
+      <c r="M44" s="45">
+        <f>MAX(K4:K49)</f>
+        <v>133512</v>
+      </c>
     </row>
     <row r="45" spans="2:56" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="21" t="s">
@@ -6667,6 +6690,37 @@
       <c r="K45" s="14">
         <f t="shared" si="0"/>
         <v>2399</v>
+      </c>
+      <c r="L45" t="s">
+        <v>65</v>
+      </c>
+      <c r="M45" s="45">
+        <f>MAX(D4:D49)</f>
+        <v>9674</v>
+      </c>
+      <c r="N45" s="45">
+        <f>MAX(E4:E49)</f>
+        <v>23461</v>
+      </c>
+      <c r="O45" s="45">
+        <f>MAX(F4:F49)</f>
+        <v>23094</v>
+      </c>
+      <c r="P45" s="45">
+        <f t="shared" ref="P45:S45" si="1">MAX(G4:G49)</f>
+        <v>30200</v>
+      </c>
+      <c r="Q45" s="45">
+        <f t="shared" si="1"/>
+        <v>26200</v>
+      </c>
+      <c r="R45" s="45">
+        <f t="shared" si="1"/>
+        <v>30200</v>
+      </c>
+      <c r="S45" s="45">
+        <f t="shared" si="1"/>
+        <v>26500</v>
       </c>
     </row>
     <row r="46" spans="2:56" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -6689,6 +6743,27 @@
         <f t="shared" si="0"/>
         <v>112</v>
       </c>
+      <c r="M46" t="s">
+        <v>67</v>
+      </c>
+      <c r="N46" t="s">
+        <v>66</v>
+      </c>
+      <c r="O46" t="s">
+        <v>66</v>
+      </c>
+      <c r="P46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>68</v>
+      </c>
+      <c r="R46" t="s">
+        <v>68</v>
+      </c>
+      <c r="S46" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="47" spans="2:56" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="21" t="s">
@@ -6710,6 +6785,27 @@
         <f t="shared" si="0"/>
         <v>518</v>
       </c>
+      <c r="M47">
+        <v>2011</v>
+      </c>
+      <c r="N47">
+        <v>2012</v>
+      </c>
+      <c r="O47">
+        <v>2013</v>
+      </c>
+      <c r="P47">
+        <v>2014</v>
+      </c>
+      <c r="Q47">
+        <v>2015</v>
+      </c>
+      <c r="R47">
+        <v>2016</v>
+      </c>
+      <c r="S47">
+        <v>2017</v>
+      </c>
     </row>
     <row r="48" spans="2:56" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="21" t="s">
@@ -6769,31 +6865,31 @@
       </c>
       <c r="C50" s="19"/>
       <c r="D50" s="16">
-        <f t="shared" ref="D50:J50" si="1">SUM(D4:D49)</f>
+        <f t="shared" ref="D50:J50" si="2">SUM(D4:D49)</f>
         <v>17731</v>
       </c>
       <c r="E50" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>53234</v>
       </c>
       <c r="F50" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>96702</v>
       </c>
       <c r="G50" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>118773</v>
       </c>
       <c r="H50" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>113923</v>
       </c>
       <c r="I50" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>159568</v>
       </c>
       <c r="J50" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>195245</v>
       </c>
       <c r="K50" s="18">

</xml_diff>